<commit_message>
Final board updates before fabrication, more & smaller vias, re-worked minor placement of parts, finalized graphics.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 5\Chem-E Car Team\McMaster_Chem-E_Car_25-26\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FFCD047-ED17-416D-BB42-49B3DDF042E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72B925FD-C9F2-4550-AA5A-00320BBD05EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{F0F3189E-63D3-4B3A-9E31-4E0939590D39}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{EA864D17-A2FA-4459-BC44-DC5D03B4B2F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="128">
   <si>
     <t>Comment</t>
   </si>
@@ -77,7 +77,7 @@
     <t>CONN HEADER VERT 2POS 2.5MM</t>
   </si>
   <si>
-    <t>AUXM, LEDB, PROP, STRM, SW, TRB</t>
+    <t>AUXM, DRVM, LEDB, PROP, SPKR, STRM, SW, TRB</t>
   </si>
   <si>
     <t>FP-B2B-XH-A_LF_SN-MFG</t>
@@ -212,12 +212,6 @@
     <t>SOP65P640X120-17N</t>
   </si>
   <si>
-    <t>SW400204-1</t>
-  </si>
-  <si>
-    <t>DRVM, SPKR</t>
-  </si>
-  <si>
     <t>61300411821</t>
   </si>
   <si>
@@ -230,7 +224,7 @@
     <t>CMP-1502-01316-4</t>
   </si>
   <si>
-    <t>Ferrite</t>
+    <t>MPZ1608S221ATA00</t>
   </si>
   <si>
     <t>Power line Ferrite Bead 220Ω @ 100MHz 2.2A DCR 0.05Ω SMD 0603</t>
@@ -245,13 +239,16 @@
     <t>CMP-08257-000028-1</t>
   </si>
   <si>
+    <t>AD623ARZ-R7</t>
+  </si>
+  <si>
+    <t>IAMP</t>
+  </si>
+  <si>
+    <t>SOIC127P600X175-8N</t>
+  </si>
+  <si>
     <t>AD623AR-REEL7</t>
-  </si>
-  <si>
-    <t>IAMP</t>
-  </si>
-  <si>
-    <t>SOIC127P600X175-8N</t>
   </si>
   <si>
     <t>1 μH</t>
@@ -821,8 +818,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA03CEC8-3076-4994-98E5-DE6AC7B1DBA8}">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8C1EFA-50FD-475B-9A22-9E84E72D5A67}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -888,7 +885,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1116,76 +1113,76 @@
         <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1193,59 +1190,59 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F20" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1253,39 +1250,39 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1293,19 +1290,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -1313,39 +1310,39 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1353,59 +1350,59 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F27" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1413,19 +1410,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
@@ -1433,16 +1430,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>122</v>
@@ -1453,41 +1450,21 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="F32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F33" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>